<commit_message>
TestInit in test case and Init tab in parent test
</commit_message>
<xml_diff>
--- a/D365SalesRvlFramework/Main.rvl.xlsx
+++ b/D365SalesRvlFramework/Main.rvl.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId2"/>
     <sheet name="GoHome" sheetId="2" r:id="rId5"/>
+    <sheet name="Init" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="66">
   <si>
     <t>Flow</t>
   </si>
@@ -210,6 +211,9 @@
   </si>
   <si>
     <t>GetProperty</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -230,7 +234,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="542">
+  <borders count="718">
     <border>
       <left/>
       <right/>
@@ -779,11 +783,187 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="542">
+  <cellXfs count="718">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -1326,6 +1506,182 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="539" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="540" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="541" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="542" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="543" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="544" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="545" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="546" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="547" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="548" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="549" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="550" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="551" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="552" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="553" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="554" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="555" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="556" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="557" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="558" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="559" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="560" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="561" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="562" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="563" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="564" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="565" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="566" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="567" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="568" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="569" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="570" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="571" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="572" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="573" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="574" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="575" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="576" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="577" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="578" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="579" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="580" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="581" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="582" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="583" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="584" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="585" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="586" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="587" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="588" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="589" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="590" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="591" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="592" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="593" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="594" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="595" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="596" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="597" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="598" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="599" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="600" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="601" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="602" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="603" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="604" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="605" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="606" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="607" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="608" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="609" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="610" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="611" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="612" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="613" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="614" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="615" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="616" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="617" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="618" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="619" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="620" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="621" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="622" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="623" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="624" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="625" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="626" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="627" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="628" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="629" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="630" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="631" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="632" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="633" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="634" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="635" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="636" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="637" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="638" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="639" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="640" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="641" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="642" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="643" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="644" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="645" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="646" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="647" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="648" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="649" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="650" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="651" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="652" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="653" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="654" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="655" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="656" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="657" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="658" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="659" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="660" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="661" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="662" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="663" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="664" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="665" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="666" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="667" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="668" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="669" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="670" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="671" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="672" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="673" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="674" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="675" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="676" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="677" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="678" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="679" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="680" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="681" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="682" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="683" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="684" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="685" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="686" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="687" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="688" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="689" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="690" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="691" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="692" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="693" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="694" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="695" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="696" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="697" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="698" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="699" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="700" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="701" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="702" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="703" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="704" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="705" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="706" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="707" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="708" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="709" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="710" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="711" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="712" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="713" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="714" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="715" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="716" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="717" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1901,4 +2257,271 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H22"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.86328125" customWidth="true"/>
+    <col min="2" max="2" width="8.86328125" customWidth="true"/>
+    <col min="3" max="3" width="12.86328125" customWidth="true"/>
+    <col min="4" max="4" width="12.86328125" customWidth="true"/>
+    <col min="5" max="5" width="12.86328125" customWidth="true"/>
+    <col min="6" max="6" width="12.86328125" customWidth="true"/>
+    <col min="7" max="7" width="12.86328125" customWidth="true"/>
+    <col min="8" max="8" width="10.86328125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="542" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="543" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="544" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="545" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="546" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="547" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="548" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="549" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="550"/>
+      <c r="B2" s="551"/>
+      <c r="C2" s="552"/>
+      <c r="D2" s="553"/>
+      <c r="E2" s="554"/>
+      <c r="F2" s="555"/>
+      <c r="G2" s="556"/>
+      <c r="H2" s="557"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="558"/>
+      <c r="B3" s="559" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="560" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="561" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="562" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="563" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="564" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="565"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="566"/>
+      <c r="B4" s="567"/>
+      <c r="C4" s="568"/>
+      <c r="D4" s="569"/>
+      <c r="E4" s="570"/>
+      <c r="F4" s="571"/>
+      <c r="G4" s="572"/>
+      <c r="H4" s="573"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="574"/>
+      <c r="B5" s="575"/>
+      <c r="C5" s="576"/>
+      <c r="D5" s="577"/>
+      <c r="E5" s="578"/>
+      <c r="F5" s="579"/>
+      <c r="G5" s="580"/>
+      <c r="H5" s="581"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="582"/>
+      <c r="B6" s="583"/>
+      <c r="C6" s="584"/>
+      <c r="D6" s="585"/>
+      <c r="E6" s="586"/>
+      <c r="F6" s="587"/>
+      <c r="G6" s="588"/>
+      <c r="H6" s="589"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="590"/>
+      <c r="B7" s="591"/>
+      <c r="C7" s="592"/>
+      <c r="D7" s="593"/>
+      <c r="E7" s="594"/>
+      <c r="F7" s="595"/>
+      <c r="G7" s="596"/>
+      <c r="H7" s="597"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="598"/>
+      <c r="B8" s="599"/>
+      <c r="C8" s="600"/>
+      <c r="D8" s="601"/>
+      <c r="E8" s="602"/>
+      <c r="F8" s="603"/>
+      <c r="G8" s="604"/>
+      <c r="H8" s="605"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="606"/>
+      <c r="B9" s="607"/>
+      <c r="C9" s="608"/>
+      <c r="D9" s="609"/>
+      <c r="E9" s="610"/>
+      <c r="F9" s="611"/>
+      <c r="G9" s="612"/>
+      <c r="H9" s="613"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="614"/>
+      <c r="B10" s="615"/>
+      <c r="C10" s="616"/>
+      <c r="D10" s="617"/>
+      <c r="E10" s="618"/>
+      <c r="F10" s="619"/>
+      <c r="G10" s="620"/>
+      <c r="H10" s="621"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="622"/>
+      <c r="B11" s="623"/>
+      <c r="C11" s="624"/>
+      <c r="D11" s="625"/>
+      <c r="E11" s="626"/>
+      <c r="F11" s="627"/>
+      <c r="G11" s="628"/>
+      <c r="H11" s="629"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="630"/>
+      <c r="B12" s="631"/>
+      <c r="C12" s="632"/>
+      <c r="D12" s="633"/>
+      <c r="E12" s="634"/>
+      <c r="F12" s="635"/>
+      <c r="G12" s="636"/>
+      <c r="H12" s="637"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="638"/>
+      <c r="B13" s="639"/>
+      <c r="C13" s="640"/>
+      <c r="D13" s="641"/>
+      <c r="E13" s="642"/>
+      <c r="F13" s="643"/>
+      <c r="G13" s="644"/>
+      <c r="H13" s="645"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="646"/>
+      <c r="B14" s="647"/>
+      <c r="C14" s="648"/>
+      <c r="D14" s="649"/>
+      <c r="E14" s="650"/>
+      <c r="F14" s="651"/>
+      <c r="G14" s="652"/>
+      <c r="H14" s="653"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="654"/>
+      <c r="B15" s="655"/>
+      <c r="C15" s="656"/>
+      <c r="D15" s="657"/>
+      <c r="E15" s="658"/>
+      <c r="F15" s="659"/>
+      <c r="G15" s="660"/>
+      <c r="H15" s="661"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="662"/>
+      <c r="B16" s="663"/>
+      <c r="C16" s="664"/>
+      <c r="D16" s="665"/>
+      <c r="E16" s="666"/>
+      <c r="F16" s="667"/>
+      <c r="G16" s="668"/>
+      <c r="H16" s="669"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="670"/>
+      <c r="B17" s="671"/>
+      <c r="C17" s="672"/>
+      <c r="D17" s="673"/>
+      <c r="E17" s="674"/>
+      <c r="F17" s="675"/>
+      <c r="G17" s="676"/>
+      <c r="H17" s="677"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="678"/>
+      <c r="B18" s="679"/>
+      <c r="C18" s="680"/>
+      <c r="D18" s="681"/>
+      <c r="E18" s="682"/>
+      <c r="F18" s="683"/>
+      <c r="G18" s="684"/>
+      <c r="H18" s="685"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="686"/>
+      <c r="B19" s="687"/>
+      <c r="C19" s="688"/>
+      <c r="D19" s="689"/>
+      <c r="E19" s="690"/>
+      <c r="F19" s="691"/>
+      <c r="G19" s="692"/>
+      <c r="H19" s="693"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="694"/>
+      <c r="B20" s="695"/>
+      <c r="C20" s="696"/>
+      <c r="D20" s="697"/>
+      <c r="E20" s="698"/>
+      <c r="F20" s="699"/>
+      <c r="G20" s="700"/>
+      <c r="H20" s="701"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="702"/>
+      <c r="B21" s="703"/>
+      <c r="C21" s="704"/>
+      <c r="D21" s="705"/>
+      <c r="E21" s="706"/>
+      <c r="F21" s="707"/>
+      <c r="G21" s="708"/>
+      <c r="H21" s="709"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="710"/>
+      <c r="B22" s="711"/>
+      <c r="C22" s="712"/>
+      <c r="D22" s="713"/>
+      <c r="E22" s="714"/>
+      <c r="F22" s="715"/>
+      <c r="G22" s="716"/>
+      <c r="H22" s="717"/>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lookup, Select Tab, Select Date
</commit_message>
<xml_diff>
--- a/D365SalesRvlFramework/Main.rvl.xlsx
+++ b/D365SalesRvlFramework/Main.rvl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="67">
   <si>
     <t>Flow</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>Birthday</t>
   </si>
 </sst>
 </file>
@@ -234,7 +237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="718">
+  <borders count="719">
     <border>
       <left/>
       <right/>
@@ -959,11 +962,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="718">
+  <cellXfs count="719">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -1682,6 +1686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="715" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="716" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="717" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="718" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1817,13 +1822,27 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="31"/>
+      <c r="A8" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>7</v>
+      </c>
       <c r="H8" s="32"/>
     </row>
     <row r="9">
@@ -2261,7 +2280,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.86328125" customWidth="true"/>
@@ -2311,216 +2330,241 @@
       <c r="H2" s="557"/>
     </row>
     <row r="3">
-      <c r="A3" s="558"/>
-      <c r="B3" s="559" t="s">
+      <c r="A3" s="718" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="560" t="s">
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="561" t="s">
+      <c r="D3" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="562" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="563" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="564" t="s">
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="558" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="559" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="560" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="561" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="562" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="563" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="564" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="565"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="566"/>
-      <c r="B4" s="567"/>
-      <c r="C4" s="568"/>
-      <c r="D4" s="569"/>
-      <c r="E4" s="570"/>
-      <c r="F4" s="571"/>
-      <c r="G4" s="572"/>
-      <c r="H4" s="573"/>
+      <c r="H4" s="565"/>
     </row>
     <row r="5">
-      <c r="A5" s="574"/>
-      <c r="B5" s="575"/>
-      <c r="C5" s="576"/>
-      <c r="D5" s="577"/>
-      <c r="E5" s="578"/>
-      <c r="F5" s="579"/>
-      <c r="G5" s="580"/>
-      <c r="H5" s="581"/>
+      <c r="A5" s="566"/>
+      <c r="B5" s="567"/>
+      <c r="C5" s="568"/>
+      <c r="D5" s="569"/>
+      <c r="E5" s="570"/>
+      <c r="F5" s="571"/>
+      <c r="G5" s="572"/>
+      <c r="H5" s="573"/>
     </row>
     <row r="6">
-      <c r="A6" s="582"/>
-      <c r="B6" s="583"/>
-      <c r="C6" s="584"/>
-      <c r="D6" s="585"/>
-      <c r="E6" s="586"/>
-      <c r="F6" s="587"/>
-      <c r="G6" s="588"/>
-      <c r="H6" s="589"/>
+      <c r="A6" s="574"/>
+      <c r="B6" s="575"/>
+      <c r="C6" s="576"/>
+      <c r="D6" s="577"/>
+      <c r="E6" s="578"/>
+      <c r="F6" s="579"/>
+      <c r="G6" s="580"/>
+      <c r="H6" s="581"/>
     </row>
     <row r="7">
-      <c r="A7" s="590"/>
-      <c r="B7" s="591"/>
-      <c r="C7" s="592"/>
-      <c r="D7" s="593"/>
-      <c r="E7" s="594"/>
-      <c r="F7" s="595"/>
-      <c r="G7" s="596"/>
-      <c r="H7" s="597"/>
+      <c r="A7" s="582"/>
+      <c r="B7" s="583"/>
+      <c r="C7" s="584"/>
+      <c r="D7" s="585"/>
+      <c r="E7" s="586"/>
+      <c r="F7" s="587"/>
+      <c r="G7" s="588"/>
+      <c r="H7" s="589"/>
     </row>
     <row r="8">
-      <c r="A8" s="598"/>
-      <c r="B8" s="599"/>
-      <c r="C8" s="600"/>
-      <c r="D8" s="601"/>
-      <c r="E8" s="602"/>
-      <c r="F8" s="603"/>
-      <c r="G8" s="604"/>
-      <c r="H8" s="605"/>
+      <c r="A8" s="590"/>
+      <c r="B8" s="591"/>
+      <c r="C8" s="592"/>
+      <c r="D8" s="593"/>
+      <c r="E8" s="594"/>
+      <c r="F8" s="595"/>
+      <c r="G8" s="596"/>
+      <c r="H8" s="597"/>
     </row>
     <row r="9">
-      <c r="A9" s="606"/>
-      <c r="B9" s="607"/>
-      <c r="C9" s="608"/>
-      <c r="D9" s="609"/>
-      <c r="E9" s="610"/>
-      <c r="F9" s="611"/>
-      <c r="G9" s="612"/>
-      <c r="H9" s="613"/>
+      <c r="A9" s="598"/>
+      <c r="B9" s="599"/>
+      <c r="C9" s="600"/>
+      <c r="D9" s="601"/>
+      <c r="E9" s="602"/>
+      <c r="F9" s="603"/>
+      <c r="G9" s="604"/>
+      <c r="H9" s="605"/>
     </row>
     <row r="10">
-      <c r="A10" s="614"/>
-      <c r="B10" s="615"/>
-      <c r="C10" s="616"/>
-      <c r="D10" s="617"/>
-      <c r="E10" s="618"/>
-      <c r="F10" s="619"/>
-      <c r="G10" s="620"/>
-      <c r="H10" s="621"/>
+      <c r="A10" s="606"/>
+      <c r="B10" s="607"/>
+      <c r="C10" s="608"/>
+      <c r="D10" s="609"/>
+      <c r="E10" s="610"/>
+      <c r="F10" s="611"/>
+      <c r="G10" s="612"/>
+      <c r="H10" s="613"/>
     </row>
     <row r="11">
-      <c r="A11" s="622"/>
-      <c r="B11" s="623"/>
-      <c r="C11" s="624"/>
-      <c r="D11" s="625"/>
-      <c r="E11" s="626"/>
-      <c r="F11" s="627"/>
-      <c r="G11" s="628"/>
-      <c r="H11" s="629"/>
+      <c r="A11" s="614"/>
+      <c r="B11" s="615"/>
+      <c r="C11" s="616"/>
+      <c r="D11" s="617"/>
+      <c r="E11" s="618"/>
+      <c r="F11" s="619"/>
+      <c r="G11" s="620"/>
+      <c r="H11" s="621"/>
     </row>
     <row r="12">
-      <c r="A12" s="630"/>
-      <c r="B12" s="631"/>
-      <c r="C12" s="632"/>
-      <c r="D12" s="633"/>
-      <c r="E12" s="634"/>
-      <c r="F12" s="635"/>
-      <c r="G12" s="636"/>
-      <c r="H12" s="637"/>
+      <c r="A12" s="622"/>
+      <c r="B12" s="623"/>
+      <c r="C12" s="624"/>
+      <c r="D12" s="625"/>
+      <c r="E12" s="626"/>
+      <c r="F12" s="627"/>
+      <c r="G12" s="628"/>
+      <c r="H12" s="629"/>
     </row>
     <row r="13">
-      <c r="A13" s="638"/>
-      <c r="B13" s="639"/>
-      <c r="C13" s="640"/>
-      <c r="D13" s="641"/>
-      <c r="E13" s="642"/>
-      <c r="F13" s="643"/>
-      <c r="G13" s="644"/>
-      <c r="H13" s="645"/>
+      <c r="A13" s="630"/>
+      <c r="B13" s="631"/>
+      <c r="C13" s="632"/>
+      <c r="D13" s="633"/>
+      <c r="E13" s="634"/>
+      <c r="F13" s="635"/>
+      <c r="G13" s="636"/>
+      <c r="H13" s="637"/>
     </row>
     <row r="14">
-      <c r="A14" s="646"/>
-      <c r="B14" s="647"/>
-      <c r="C14" s="648"/>
-      <c r="D14" s="649"/>
-      <c r="E14" s="650"/>
-      <c r="F14" s="651"/>
-      <c r="G14" s="652"/>
-      <c r="H14" s="653"/>
+      <c r="A14" s="638"/>
+      <c r="B14" s="639"/>
+      <c r="C14" s="640"/>
+      <c r="D14" s="641"/>
+      <c r="E14" s="642"/>
+      <c r="F14" s="643"/>
+      <c r="G14" s="644"/>
+      <c r="H14" s="645"/>
     </row>
     <row r="15">
-      <c r="A15" s="654"/>
-      <c r="B15" s="655"/>
-      <c r="C15" s="656"/>
-      <c r="D15" s="657"/>
-      <c r="E15" s="658"/>
-      <c r="F15" s="659"/>
-      <c r="G15" s="660"/>
-      <c r="H15" s="661"/>
+      <c r="A15" s="646"/>
+      <c r="B15" s="647"/>
+      <c r="C15" s="648"/>
+      <c r="D15" s="649"/>
+      <c r="E15" s="650"/>
+      <c r="F15" s="651"/>
+      <c r="G15" s="652"/>
+      <c r="H15" s="653"/>
     </row>
     <row r="16">
-      <c r="A16" s="662"/>
-      <c r="B16" s="663"/>
-      <c r="C16" s="664"/>
-      <c r="D16" s="665"/>
-      <c r="E16" s="666"/>
-      <c r="F16" s="667"/>
-      <c r="G16" s="668"/>
-      <c r="H16" s="669"/>
+      <c r="A16" s="654"/>
+      <c r="B16" s="655"/>
+      <c r="C16" s="656"/>
+      <c r="D16" s="657"/>
+      <c r="E16" s="658"/>
+      <c r="F16" s="659"/>
+      <c r="G16" s="660"/>
+      <c r="H16" s="661"/>
     </row>
     <row r="17">
-      <c r="A17" s="670"/>
-      <c r="B17" s="671"/>
-      <c r="C17" s="672"/>
-      <c r="D17" s="673"/>
-      <c r="E17" s="674"/>
-      <c r="F17" s="675"/>
-      <c r="G17" s="676"/>
-      <c r="H17" s="677"/>
+      <c r="A17" s="662"/>
+      <c r="B17" s="663"/>
+      <c r="C17" s="664"/>
+      <c r="D17" s="665"/>
+      <c r="E17" s="666"/>
+      <c r="F17" s="667"/>
+      <c r="G17" s="668"/>
+      <c r="H17" s="669"/>
     </row>
     <row r="18">
-      <c r="A18" s="678"/>
-      <c r="B18" s="679"/>
-      <c r="C18" s="680"/>
-      <c r="D18" s="681"/>
-      <c r="E18" s="682"/>
-      <c r="F18" s="683"/>
-      <c r="G18" s="684"/>
-      <c r="H18" s="685"/>
+      <c r="A18" s="670"/>
+      <c r="B18" s="671"/>
+      <c r="C18" s="672"/>
+      <c r="D18" s="673"/>
+      <c r="E18" s="674"/>
+      <c r="F18" s="675"/>
+      <c r="G18" s="676"/>
+      <c r="H18" s="677"/>
     </row>
     <row r="19">
-      <c r="A19" s="686"/>
-      <c r="B19" s="687"/>
-      <c r="C19" s="688"/>
-      <c r="D19" s="689"/>
-      <c r="E19" s="690"/>
-      <c r="F19" s="691"/>
-      <c r="G19" s="692"/>
-      <c r="H19" s="693"/>
+      <c r="A19" s="678"/>
+      <c r="B19" s="679"/>
+      <c r="C19" s="680"/>
+      <c r="D19" s="681"/>
+      <c r="E19" s="682"/>
+      <c r="F19" s="683"/>
+      <c r="G19" s="684"/>
+      <c r="H19" s="685"/>
     </row>
     <row r="20">
-      <c r="A20" s="694"/>
-      <c r="B20" s="695"/>
-      <c r="C20" s="696"/>
-      <c r="D20" s="697"/>
-      <c r="E20" s="698"/>
-      <c r="F20" s="699"/>
-      <c r="G20" s="700"/>
-      <c r="H20" s="701"/>
+      <c r="A20" s="686"/>
+      <c r="B20" s="687"/>
+      <c r="C20" s="688"/>
+      <c r="D20" s="689"/>
+      <c r="E20" s="690"/>
+      <c r="F20" s="691"/>
+      <c r="G20" s="692"/>
+      <c r="H20" s="693"/>
     </row>
     <row r="21">
-      <c r="A21" s="702"/>
-      <c r="B21" s="703"/>
-      <c r="C21" s="704"/>
-      <c r="D21" s="705"/>
-      <c r="E21" s="706"/>
-      <c r="F21" s="707"/>
-      <c r="G21" s="708"/>
-      <c r="H21" s="709"/>
+      <c r="A21" s="694"/>
+      <c r="B21" s="695"/>
+      <c r="C21" s="696"/>
+      <c r="D21" s="697"/>
+      <c r="E21" s="698"/>
+      <c r="F21" s="699"/>
+      <c r="G21" s="700"/>
+      <c r="H21" s="701"/>
     </row>
     <row r="22">
-      <c r="A22" s="710"/>
-      <c r="B22" s="711"/>
-      <c r="C22" s="712"/>
-      <c r="D22" s="713"/>
-      <c r="E22" s="714"/>
-      <c r="F22" s="715"/>
-      <c r="G22" s="716"/>
-      <c r="H22" s="717"/>
+      <c r="A22" s="702"/>
+      <c r="B22" s="703"/>
+      <c r="C22" s="704"/>
+      <c r="D22" s="705"/>
+      <c r="E22" s="706"/>
+      <c r="F22" s="707"/>
+      <c r="G22" s="708"/>
+      <c r="H22" s="709"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="710"/>
+      <c r="B23" s="711"/>
+      <c r="C23" s="712"/>
+      <c r="D23" s="713"/>
+      <c r="E23" s="714"/>
+      <c r="F23" s="715"/>
+      <c r="G23" s="716"/>
+      <c r="H23" s="717"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
Docs for new actions
</commit_message>
<xml_diff>
--- a/D365SalesRvlFramework/Main.rvl.xlsx
+++ b/D365SalesRvlFramework/Main.rvl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="67">
   <si>
     <t>Flow</t>
   </si>
@@ -237,7 +237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="719">
+  <borders count="721">
     <border>
       <left/>
       <right/>
@@ -963,11 +963,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="719">
+  <cellXfs count="721">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -1687,6 +1689,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="716" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="717" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="718" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="719" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="720" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>